<commit_message>
handle opened xlsx file
</commit_message>
<xml_diff>
--- a/db/test.xlsx
+++ b/db/test.xlsx
@@ -1,37 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u130035\Desktop\pc-status-website\pc-status-website\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5D1EAB-6826-400F-8ECC-F21A689950A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>שם מלא</t>
+  </si>
+  <si>
+    <t>תאריך כניסת מחשב</t>
+  </si>
+  <si>
+    <t>הפעולה הנדרשת</t>
+  </si>
+  <si>
+    <t>פרמוט לרשת</t>
+  </si>
+  <si>
+    <t>מספר סריאלי</t>
+  </si>
+  <si>
+    <t>סגמנט במשרד</t>
+  </si>
+  <si>
+    <t>יחידה</t>
+  </si>
+  <si>
+    <t>מספר אישי/ת.ז</t>
+  </si>
+  <si>
+    <t>מייל אזרחי</t>
+  </si>
+  <si>
+    <t>טלפון אזרחי</t>
+  </si>
+  <si>
+    <t>הערות</t>
+  </si>
+  <si>
+    <t>סטטוס</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +93,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,141 +417,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>שם מלא</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>תאריך כניסת מחשב</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>הפעולה הנדרשת</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>פרמוט לרשת</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>מספר סריאלי</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>סגמנט במשרד</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>יחידה</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>מספר אישי/ת.ז</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>מייל אזרחי</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>טלפון אזרחי</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>הערות</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>סטטוס</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>נאור אור ציון</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2023-10-20</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>תיקון תקלה חמורה</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2UA12345</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>בסמח</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>naororzion101@gmail.com</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0501234567</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>אין</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>מחשבים שלא טופלו</t>
-        </is>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move freely between sections
</commit_message>
<xml_diff>
--- a/db/test.xlsx
+++ b/db/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,7 +550,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>נמחקו</t>
+          <t>מחשבים שלא טופלו</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>נמחקו</t>
+          <t>מחשבים שטופלו ונלקחו</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -674,6 +674,65 @@
       <c r="M4" t="inlineStr">
         <is>
           <t>ACYDBNiRa7E-B6QBh5aq1oWeLHR-OBuIDTBKAQiPS1tTSeGUUzRH0Fe4_MNUDpy-DvSisbM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>אלדד עזוז</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>הכנסה לדומיין</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2UA24222</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1212</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>בסמח</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>9996333</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>eldad@gmail.com</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>502361254</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>מחשבים שטופלו ונלקחו</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>ACYDBNiG4l0vuauSyQwWZACPpzh8iDZLIfRlzvKrqVv4HgeEZEIz5MhWbVMoxJVy6XDDDis</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
don't allow duplicate responses
</commit_message>
<xml_diff>
--- a/db/test.xlsx
+++ b/db/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u130035\Desktop\pc-status-website\pc-status-website\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4B43E1-C7F4-4997-A0DA-F01513826E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241E1D6-1C67-41CF-8CE5-90E674BE1B6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>שם מלא</t>
   </si>
@@ -70,15 +70,27 @@
     <t>הכנסה לדומיין</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>2UA12345</t>
   </si>
   <si>
+    <t>333</t>
+  </si>
+  <si>
     <t>בסמח</t>
   </si>
   <si>
+    <t>132456789</t>
+  </si>
+  <si>
     <t>naororzion101@gmail.com</t>
   </si>
   <si>
+    <t>502223544</t>
+  </si>
+  <si>
     <t>אין</t>
   </si>
   <si>
@@ -94,15 +106,27 @@
     <t>2023-10-17</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>3UA12345</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
     <t>לוטם</t>
   </si>
   <si>
+    <t>123123123</t>
+  </si>
+  <si>
     <t>shayy@gmail.com</t>
   </si>
   <si>
+    <t>502221234</t>
+  </si>
+  <si>
     <t>ACYDBNj5FvHeBJa9vLyd5T2WPs2Mz_tT5_jAgi0n85vMZVLjmxSbKtdVCgFSrRVqGVhHL04</t>
   </si>
   <si>
@@ -112,15 +136,27 @@
     <t>2023-10-18</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>2UA4532</t>
   </si>
   <si>
+    <t>454</t>
+  </si>
+  <si>
     <t>מצפ"ן</t>
   </si>
   <si>
+    <t>987654321</t>
+  </si>
+  <si>
     <t>itamar@gmail.com</t>
   </si>
   <si>
+    <t>507891234</t>
+  </si>
+  <si>
     <t>ACYDBNiRa7E-B6QBh5aq1oWeLHR-OBuIDTBKAQiPS1tTSeGUUzRH0Fe4_MNUDpy-DvSisbM</t>
   </si>
   <si>
@@ -130,7 +166,16 @@
     <t>2UA24222</t>
   </si>
   <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>9996333</t>
+  </si>
+  <si>
     <t>eldad@gmail.com</t>
+  </si>
+  <si>
+    <t>502361254</t>
   </si>
   <si>
     <t>מחשבים שטופלו ונלקחו</t>
@@ -502,7 +547,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,158 +603,158 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="D2" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2">
-        <v>333</v>
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2">
-        <v>132456789</v>
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2">
-        <v>502223544</v>
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>28</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="F3">
-        <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>123123123</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>502221234</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
-        <v>7</v>
+      <c r="D4" t="s">
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>454</v>
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4">
-        <v>987654321</v>
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4">
-        <v>507891234</v>
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>2</v>
+      <c r="D5" t="s">
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5">
-        <v>1212</v>
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5">
-        <v>9996333</v>
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5">
-        <v>502361254</v>
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add favicon and logo
</commit_message>
<xml_diff>
--- a/db/test.xlsx
+++ b/db/test.xlsx
@@ -550,7 +550,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>מחשבים שטופלו ולא נלקחו</t>
+          <t>מחשבים שטופלו ונלקחו</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>מחשבים שטופלו ולא נלקחו</t>
+          <t>מחשבים שלא טופלו</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">

</xml_diff>